<commit_message>
Updated Python to 3.12
</commit_message>
<xml_diff>
--- a/gridGenerator/Timetable.xlsx
+++ b/gridGenerator/Timetable.xlsx
@@ -1252,18 +1252,18 @@
       <c r="AU3" s="23" t="n"/>
       <c r="AV3" s="23" t="n"/>
       <c r="AW3" s="24" t="n"/>
-      <c r="AX3" s="22" t="n"/>
-      <c r="AY3" s="23" t="n"/>
-      <c r="AZ3" s="23" t="n"/>
-      <c r="BA3" s="23" t="n"/>
-      <c r="BB3" s="23" t="n"/>
-      <c r="BC3" s="23" t="n"/>
-      <c r="BD3" s="23" t="n"/>
-      <c r="BE3" s="23" t="n"/>
-      <c r="BF3" s="23" t="n"/>
-      <c r="BG3" s="23" t="n"/>
-      <c r="BH3" s="23" t="n"/>
-      <c r="BI3" s="24" t="n"/>
+      <c r="AX3" s="25" t="n"/>
+      <c r="AY3" s="26" t="n"/>
+      <c r="AZ3" s="26" t="n"/>
+      <c r="BA3" s="26" t="n"/>
+      <c r="BB3" s="26" t="n"/>
+      <c r="BC3" s="26" t="n"/>
+      <c r="BD3" s="26" t="n"/>
+      <c r="BE3" s="26" t="n"/>
+      <c r="BF3" s="26" t="n"/>
+      <c r="BG3" s="26" t="n"/>
+      <c r="BH3" s="26" t="n"/>
+      <c r="BI3" s="27" t="n"/>
       <c r="BJ3" s="22" t="n"/>
       <c r="BK3" s="23" t="n"/>
       <c r="BL3" s="23" t="n"/>
@@ -1427,27 +1427,27 @@
       <c r="W4" s="23" t="n"/>
       <c r="X4" s="23" t="n"/>
       <c r="Y4" s="24" t="n"/>
-      <c r="Z4" s="25" t="n"/>
-      <c r="AA4" s="26" t="n"/>
-      <c r="AB4" s="26" t="n"/>
-      <c r="AC4" s="26" t="n"/>
-      <c r="AD4" s="26" t="n"/>
-      <c r="AE4" s="26" t="n"/>
-      <c r="AF4" s="26" t="n"/>
-      <c r="AG4" s="26" t="n"/>
-      <c r="AH4" s="26" t="n"/>
-      <c r="AI4" s="26" t="n"/>
-      <c r="AJ4" s="26" t="n"/>
-      <c r="AK4" s="27" t="n"/>
-      <c r="AL4" s="25" t="n"/>
-      <c r="AM4" s="26" t="n"/>
-      <c r="AN4" s="26" t="n"/>
-      <c r="AO4" s="26" t="n"/>
-      <c r="AP4" s="26" t="n"/>
-      <c r="AQ4" s="26" t="n"/>
-      <c r="AR4" s="26" t="n"/>
-      <c r="AS4" s="26" t="n"/>
-      <c r="AT4" s="26" t="n"/>
+      <c r="Z4" s="22" t="n"/>
+      <c r="AA4" s="23" t="n"/>
+      <c r="AB4" s="23" t="n"/>
+      <c r="AC4" s="23" t="n"/>
+      <c r="AD4" s="23" t="n"/>
+      <c r="AE4" s="23" t="n"/>
+      <c r="AF4" s="23" t="n"/>
+      <c r="AG4" s="23" t="n"/>
+      <c r="AH4" s="23" t="n"/>
+      <c r="AI4" s="23" t="n"/>
+      <c r="AJ4" s="23" t="n"/>
+      <c r="AK4" s="24" t="n"/>
+      <c r="AL4" s="22" t="n"/>
+      <c r="AM4" s="23" t="n"/>
+      <c r="AN4" s="23" t="n"/>
+      <c r="AO4" s="23" t="n"/>
+      <c r="AP4" s="23" t="n"/>
+      <c r="AQ4" s="23" t="n"/>
+      <c r="AR4" s="23" t="n"/>
+      <c r="AS4" s="23" t="n"/>
+      <c r="AT4" s="23" t="n"/>
       <c r="AU4" s="23" t="n"/>
       <c r="AV4" s="23" t="n"/>
       <c r="AW4" s="24" t="n"/>
@@ -1541,45 +1541,45 @@
       <c r="EG4" s="23" t="n"/>
       <c r="EH4" s="23" t="n"/>
       <c r="EI4" s="23" t="n"/>
-      <c r="EJ4" s="26" t="n"/>
-      <c r="EK4" s="26" t="n"/>
-      <c r="EL4" s="26" t="n"/>
-      <c r="EM4" s="26" t="n"/>
-      <c r="EN4" s="26" t="n"/>
-      <c r="EO4" s="27" t="n"/>
-      <c r="EP4" s="25" t="n"/>
-      <c r="EQ4" s="26" t="n"/>
-      <c r="ER4" s="26" t="n"/>
-      <c r="ES4" s="26" t="n"/>
-      <c r="ET4" s="26" t="n"/>
-      <c r="EU4" s="26" t="n"/>
-      <c r="EV4" s="26" t="n"/>
-      <c r="EW4" s="26" t="n"/>
-      <c r="EX4" s="26" t="n"/>
-      <c r="EY4" s="26" t="n"/>
-      <c r="EZ4" s="26" t="n"/>
-      <c r="FA4" s="27" t="n"/>
-      <c r="FB4" s="25" t="n"/>
-      <c r="FC4" s="26" t="n"/>
-      <c r="FD4" s="26" t="n"/>
-      <c r="FE4" s="26" t="n"/>
-      <c r="FF4" s="26" t="n"/>
-      <c r="FG4" s="26" t="n"/>
-      <c r="FH4" s="26" t="n"/>
-      <c r="FI4" s="26" t="n"/>
-      <c r="FJ4" s="26" t="n"/>
-      <c r="FK4" s="26" t="n"/>
-      <c r="FL4" s="26" t="n"/>
-      <c r="FM4" s="27" t="n"/>
-      <c r="FN4" s="25" t="n"/>
-      <c r="FO4" s="26" t="n"/>
-      <c r="FP4" s="26" t="n"/>
-      <c r="FQ4" s="26" t="n"/>
-      <c r="FR4" s="26" t="n"/>
-      <c r="FS4" s="26" t="n"/>
-      <c r="FT4" s="26" t="n"/>
-      <c r="FU4" s="26" t="n"/>
-      <c r="FV4" s="26" t="n"/>
+      <c r="EJ4" s="23" t="n"/>
+      <c r="EK4" s="23" t="n"/>
+      <c r="EL4" s="23" t="n"/>
+      <c r="EM4" s="23" t="n"/>
+      <c r="EN4" s="23" t="n"/>
+      <c r="EO4" s="24" t="n"/>
+      <c r="EP4" s="22" t="n"/>
+      <c r="EQ4" s="23" t="n"/>
+      <c r="ER4" s="23" t="n"/>
+      <c r="ES4" s="23" t="n"/>
+      <c r="ET4" s="23" t="n"/>
+      <c r="EU4" s="23" t="n"/>
+      <c r="EV4" s="23" t="n"/>
+      <c r="EW4" s="23" t="n"/>
+      <c r="EX4" s="23" t="n"/>
+      <c r="EY4" s="23" t="n"/>
+      <c r="EZ4" s="23" t="n"/>
+      <c r="FA4" s="24" t="n"/>
+      <c r="FB4" s="22" t="n"/>
+      <c r="FC4" s="23" t="n"/>
+      <c r="FD4" s="23" t="n"/>
+      <c r="FE4" s="23" t="n"/>
+      <c r="FF4" s="23" t="n"/>
+      <c r="FG4" s="23" t="n"/>
+      <c r="FH4" s="23" t="n"/>
+      <c r="FI4" s="23" t="n"/>
+      <c r="FJ4" s="23" t="n"/>
+      <c r="FK4" s="23" t="n"/>
+      <c r="FL4" s="23" t="n"/>
+      <c r="FM4" s="24" t="n"/>
+      <c r="FN4" s="22" t="n"/>
+      <c r="FO4" s="23" t="n"/>
+      <c r="FP4" s="23" t="n"/>
+      <c r="FQ4" s="23" t="n"/>
+      <c r="FR4" s="23" t="n"/>
+      <c r="FS4" s="23" t="n"/>
+      <c r="FT4" s="23" t="n"/>
+      <c r="FU4" s="23" t="n"/>
+      <c r="FV4" s="23" t="n"/>
       <c r="FW4" s="23" t="n"/>
       <c r="FX4" s="23" t="n"/>
       <c r="FY4" s="24" t="n"/>
@@ -1638,36 +1638,36 @@
       <c r="AI5" s="23" t="n"/>
       <c r="AJ5" s="23" t="n"/>
       <c r="AK5" s="24" t="n"/>
-      <c r="AL5" s="25" t="n"/>
-      <c r="AM5" s="26" t="n"/>
-      <c r="AN5" s="26" t="n"/>
-      <c r="AO5" s="26" t="n"/>
-      <c r="AP5" s="26" t="n"/>
-      <c r="AQ5" s="26" t="n"/>
-      <c r="AR5" s="26" t="n"/>
-      <c r="AS5" s="26" t="n"/>
-      <c r="AT5" s="26" t="n"/>
-      <c r="AU5" s="26" t="n"/>
-      <c r="AV5" s="26" t="n"/>
-      <c r="AW5" s="27" t="n"/>
-      <c r="AX5" s="25" t="n"/>
-      <c r="AY5" s="26" t="n"/>
-      <c r="AZ5" s="26" t="n"/>
-      <c r="BA5" s="26" t="n"/>
-      <c r="BB5" s="26" t="n"/>
-      <c r="BC5" s="26" t="n"/>
-      <c r="BD5" s="26" t="n"/>
-      <c r="BE5" s="26" t="n"/>
-      <c r="BF5" s="26" t="n"/>
-      <c r="BG5" s="26" t="n"/>
-      <c r="BH5" s="26" t="n"/>
-      <c r="BI5" s="27" t="n"/>
-      <c r="BJ5" s="25" t="n"/>
-      <c r="BK5" s="26" t="n"/>
-      <c r="BL5" s="26" t="n"/>
-      <c r="BM5" s="26" t="n"/>
-      <c r="BN5" s="26" t="n"/>
-      <c r="BO5" s="26" t="n"/>
+      <c r="AL5" s="22" t="n"/>
+      <c r="AM5" s="23" t="n"/>
+      <c r="AN5" s="23" t="n"/>
+      <c r="AO5" s="23" t="n"/>
+      <c r="AP5" s="23" t="n"/>
+      <c r="AQ5" s="23" t="n"/>
+      <c r="AR5" s="23" t="n"/>
+      <c r="AS5" s="23" t="n"/>
+      <c r="AT5" s="23" t="n"/>
+      <c r="AU5" s="23" t="n"/>
+      <c r="AV5" s="23" t="n"/>
+      <c r="AW5" s="24" t="n"/>
+      <c r="AX5" s="22" t="n"/>
+      <c r="AY5" s="23" t="n"/>
+      <c r="AZ5" s="23" t="n"/>
+      <c r="BA5" s="23" t="n"/>
+      <c r="BB5" s="23" t="n"/>
+      <c r="BC5" s="23" t="n"/>
+      <c r="BD5" s="23" t="n"/>
+      <c r="BE5" s="23" t="n"/>
+      <c r="BF5" s="23" t="n"/>
+      <c r="BG5" s="23" t="n"/>
+      <c r="BH5" s="23" t="n"/>
+      <c r="BI5" s="24" t="n"/>
+      <c r="BJ5" s="22" t="n"/>
+      <c r="BK5" s="23" t="n"/>
+      <c r="BL5" s="23" t="n"/>
+      <c r="BM5" s="23" t="n"/>
+      <c r="BN5" s="23" t="n"/>
+      <c r="BO5" s="23" t="n"/>
       <c r="BP5" s="23" t="n"/>
       <c r="BQ5" s="23" t="n"/>
       <c r="BR5" s="23" t="n"/>
@@ -1710,20 +1710,20 @@
       <c r="DC5" s="23" t="n"/>
       <c r="DD5" s="23" t="n"/>
       <c r="DE5" s="24" t="n"/>
-      <c r="DF5" s="25" t="n"/>
-      <c r="DG5" s="26" t="n"/>
-      <c r="DH5" s="26" t="n"/>
-      <c r="DI5" s="26" t="n"/>
-      <c r="DJ5" s="26" t="n"/>
-      <c r="DK5" s="26" t="n"/>
-      <c r="DL5" s="26" t="n"/>
-      <c r="DM5" s="26" t="n"/>
-      <c r="DN5" s="26" t="n"/>
-      <c r="DO5" s="26" t="n"/>
-      <c r="DP5" s="26" t="n"/>
-      <c r="DQ5" s="27" t="n"/>
-      <c r="DR5" s="25" t="n"/>
-      <c r="DS5" s="26" t="n"/>
+      <c r="DF5" s="22" t="n"/>
+      <c r="DG5" s="23" t="n"/>
+      <c r="DH5" s="23" t="n"/>
+      <c r="DI5" s="23" t="n"/>
+      <c r="DJ5" s="23" t="n"/>
+      <c r="DK5" s="23" t="n"/>
+      <c r="DL5" s="23" t="n"/>
+      <c r="DM5" s="23" t="n"/>
+      <c r="DN5" s="23" t="n"/>
+      <c r="DO5" s="23" t="n"/>
+      <c r="DP5" s="23" t="n"/>
+      <c r="DQ5" s="24" t="n"/>
+      <c r="DR5" s="22" t="n"/>
+      <c r="DS5" s="23" t="n"/>
       <c r="DT5" s="23" t="n"/>
       <c r="DU5" s="23" t="n"/>
       <c r="DV5" s="23" t="n"/>
@@ -1825,27 +1825,27 @@
       <c r="W6" s="23" t="n"/>
       <c r="X6" s="23" t="n"/>
       <c r="Y6" s="24" t="n"/>
-      <c r="Z6" s="25" t="n"/>
-      <c r="AA6" s="26" t="n"/>
-      <c r="AB6" s="26" t="n"/>
-      <c r="AC6" s="26" t="n"/>
-      <c r="AD6" s="26" t="n"/>
-      <c r="AE6" s="26" t="n"/>
-      <c r="AF6" s="26" t="n"/>
-      <c r="AG6" s="26" t="n"/>
-      <c r="AH6" s="26" t="n"/>
-      <c r="AI6" s="26" t="n"/>
-      <c r="AJ6" s="26" t="n"/>
-      <c r="AK6" s="27" t="n"/>
-      <c r="AL6" s="25" t="n"/>
-      <c r="AM6" s="26" t="n"/>
-      <c r="AN6" s="26" t="n"/>
-      <c r="AO6" s="26" t="n"/>
-      <c r="AP6" s="26" t="n"/>
-      <c r="AQ6" s="26" t="n"/>
-      <c r="AR6" s="26" t="n"/>
-      <c r="AS6" s="26" t="n"/>
-      <c r="AT6" s="26" t="n"/>
+      <c r="Z6" s="22" t="n"/>
+      <c r="AA6" s="23" t="n"/>
+      <c r="AB6" s="23" t="n"/>
+      <c r="AC6" s="23" t="n"/>
+      <c r="AD6" s="23" t="n"/>
+      <c r="AE6" s="23" t="n"/>
+      <c r="AF6" s="23" t="n"/>
+      <c r="AG6" s="23" t="n"/>
+      <c r="AH6" s="23" t="n"/>
+      <c r="AI6" s="23" t="n"/>
+      <c r="AJ6" s="23" t="n"/>
+      <c r="AK6" s="24" t="n"/>
+      <c r="AL6" s="22" t="n"/>
+      <c r="AM6" s="23" t="n"/>
+      <c r="AN6" s="23" t="n"/>
+      <c r="AO6" s="23" t="n"/>
+      <c r="AP6" s="23" t="n"/>
+      <c r="AQ6" s="23" t="n"/>
+      <c r="AR6" s="23" t="n"/>
+      <c r="AS6" s="23" t="n"/>
+      <c r="AT6" s="23" t="n"/>
       <c r="AU6" s="23" t="n"/>
       <c r="AV6" s="23" t="n"/>
       <c r="AW6" s="24" t="n"/>
@@ -1939,45 +1939,45 @@
       <c r="EG6" s="23" t="n"/>
       <c r="EH6" s="23" t="n"/>
       <c r="EI6" s="23" t="n"/>
-      <c r="EJ6" s="26" t="n"/>
-      <c r="EK6" s="26" t="n"/>
-      <c r="EL6" s="26" t="n"/>
-      <c r="EM6" s="26" t="n"/>
-      <c r="EN6" s="26" t="n"/>
-      <c r="EO6" s="27" t="n"/>
-      <c r="EP6" s="25" t="n"/>
-      <c r="EQ6" s="26" t="n"/>
-      <c r="ER6" s="26" t="n"/>
-      <c r="ES6" s="26" t="n"/>
-      <c r="ET6" s="26" t="n"/>
-      <c r="EU6" s="26" t="n"/>
-      <c r="EV6" s="26" t="n"/>
-      <c r="EW6" s="26" t="n"/>
-      <c r="EX6" s="26" t="n"/>
-      <c r="EY6" s="26" t="n"/>
-      <c r="EZ6" s="26" t="n"/>
-      <c r="FA6" s="27" t="n"/>
-      <c r="FB6" s="25" t="n"/>
-      <c r="FC6" s="26" t="n"/>
-      <c r="FD6" s="26" t="n"/>
-      <c r="FE6" s="26" t="n"/>
-      <c r="FF6" s="26" t="n"/>
-      <c r="FG6" s="26" t="n"/>
-      <c r="FH6" s="26" t="n"/>
-      <c r="FI6" s="26" t="n"/>
-      <c r="FJ6" s="26" t="n"/>
-      <c r="FK6" s="26" t="n"/>
-      <c r="FL6" s="26" t="n"/>
-      <c r="FM6" s="27" t="n"/>
-      <c r="FN6" s="25" t="n"/>
-      <c r="FO6" s="26" t="n"/>
-      <c r="FP6" s="26" t="n"/>
-      <c r="FQ6" s="26" t="n"/>
-      <c r="FR6" s="26" t="n"/>
-      <c r="FS6" s="26" t="n"/>
-      <c r="FT6" s="26" t="n"/>
-      <c r="FU6" s="26" t="n"/>
-      <c r="FV6" s="26" t="n"/>
+      <c r="EJ6" s="23" t="n"/>
+      <c r="EK6" s="23" t="n"/>
+      <c r="EL6" s="23" t="n"/>
+      <c r="EM6" s="23" t="n"/>
+      <c r="EN6" s="23" t="n"/>
+      <c r="EO6" s="24" t="n"/>
+      <c r="EP6" s="22" t="n"/>
+      <c r="EQ6" s="23" t="n"/>
+      <c r="ER6" s="23" t="n"/>
+      <c r="ES6" s="23" t="n"/>
+      <c r="ET6" s="23" t="n"/>
+      <c r="EU6" s="23" t="n"/>
+      <c r="EV6" s="23" t="n"/>
+      <c r="EW6" s="23" t="n"/>
+      <c r="EX6" s="23" t="n"/>
+      <c r="EY6" s="23" t="n"/>
+      <c r="EZ6" s="23" t="n"/>
+      <c r="FA6" s="24" t="n"/>
+      <c r="FB6" s="22" t="n"/>
+      <c r="FC6" s="23" t="n"/>
+      <c r="FD6" s="23" t="n"/>
+      <c r="FE6" s="23" t="n"/>
+      <c r="FF6" s="23" t="n"/>
+      <c r="FG6" s="23" t="n"/>
+      <c r="FH6" s="23" t="n"/>
+      <c r="FI6" s="23" t="n"/>
+      <c r="FJ6" s="23" t="n"/>
+      <c r="FK6" s="23" t="n"/>
+      <c r="FL6" s="23" t="n"/>
+      <c r="FM6" s="24" t="n"/>
+      <c r="FN6" s="22" t="n"/>
+      <c r="FO6" s="23" t="n"/>
+      <c r="FP6" s="23" t="n"/>
+      <c r="FQ6" s="23" t="n"/>
+      <c r="FR6" s="23" t="n"/>
+      <c r="FS6" s="23" t="n"/>
+      <c r="FT6" s="23" t="n"/>
+      <c r="FU6" s="23" t="n"/>
+      <c r="FV6" s="23" t="n"/>
       <c r="FW6" s="23" t="n"/>
       <c r="FX6" s="23" t="n"/>
       <c r="FY6" s="24" t="n"/>
@@ -2036,36 +2036,36 @@
       <c r="AI7" s="23" t="n"/>
       <c r="AJ7" s="23" t="n"/>
       <c r="AK7" s="24" t="n"/>
-      <c r="AL7" s="25" t="n"/>
-      <c r="AM7" s="26" t="n"/>
-      <c r="AN7" s="26" t="n"/>
-      <c r="AO7" s="26" t="n"/>
-      <c r="AP7" s="26" t="n"/>
-      <c r="AQ7" s="26" t="n"/>
-      <c r="AR7" s="26" t="n"/>
-      <c r="AS7" s="26" t="n"/>
-      <c r="AT7" s="26" t="n"/>
-      <c r="AU7" s="26" t="n"/>
-      <c r="AV7" s="26" t="n"/>
-      <c r="AW7" s="27" t="n"/>
-      <c r="AX7" s="25" t="n"/>
-      <c r="AY7" s="26" t="n"/>
-      <c r="AZ7" s="26" t="n"/>
-      <c r="BA7" s="26" t="n"/>
-      <c r="BB7" s="26" t="n"/>
-      <c r="BC7" s="26" t="n"/>
-      <c r="BD7" s="26" t="n"/>
-      <c r="BE7" s="26" t="n"/>
-      <c r="BF7" s="26" t="n"/>
-      <c r="BG7" s="26" t="n"/>
-      <c r="BH7" s="26" t="n"/>
-      <c r="BI7" s="27" t="n"/>
-      <c r="BJ7" s="25" t="n"/>
-      <c r="BK7" s="26" t="n"/>
-      <c r="BL7" s="26" t="n"/>
-      <c r="BM7" s="26" t="n"/>
-      <c r="BN7" s="26" t="n"/>
-      <c r="BO7" s="26" t="n"/>
+      <c r="AL7" s="22" t="n"/>
+      <c r="AM7" s="23" t="n"/>
+      <c r="AN7" s="23" t="n"/>
+      <c r="AO7" s="23" t="n"/>
+      <c r="AP7" s="23" t="n"/>
+      <c r="AQ7" s="23" t="n"/>
+      <c r="AR7" s="23" t="n"/>
+      <c r="AS7" s="23" t="n"/>
+      <c r="AT7" s="23" t="n"/>
+      <c r="AU7" s="23" t="n"/>
+      <c r="AV7" s="23" t="n"/>
+      <c r="AW7" s="24" t="n"/>
+      <c r="AX7" s="22" t="n"/>
+      <c r="AY7" s="23" t="n"/>
+      <c r="AZ7" s="23" t="n"/>
+      <c r="BA7" s="23" t="n"/>
+      <c r="BB7" s="23" t="n"/>
+      <c r="BC7" s="23" t="n"/>
+      <c r="BD7" s="23" t="n"/>
+      <c r="BE7" s="23" t="n"/>
+      <c r="BF7" s="23" t="n"/>
+      <c r="BG7" s="23" t="n"/>
+      <c r="BH7" s="23" t="n"/>
+      <c r="BI7" s="24" t="n"/>
+      <c r="BJ7" s="22" t="n"/>
+      <c r="BK7" s="23" t="n"/>
+      <c r="BL7" s="23" t="n"/>
+      <c r="BM7" s="23" t="n"/>
+      <c r="BN7" s="23" t="n"/>
+      <c r="BO7" s="23" t="n"/>
       <c r="BP7" s="23" t="n"/>
       <c r="BQ7" s="23" t="n"/>
       <c r="BR7" s="23" t="n"/>
@@ -2108,20 +2108,20 @@
       <c r="DC7" s="23" t="n"/>
       <c r="DD7" s="23" t="n"/>
       <c r="DE7" s="24" t="n"/>
-      <c r="DF7" s="25" t="n"/>
-      <c r="DG7" s="26" t="n"/>
-      <c r="DH7" s="26" t="n"/>
-      <c r="DI7" s="26" t="n"/>
-      <c r="DJ7" s="26" t="n"/>
-      <c r="DK7" s="26" t="n"/>
-      <c r="DL7" s="26" t="n"/>
-      <c r="DM7" s="26" t="n"/>
-      <c r="DN7" s="26" t="n"/>
-      <c r="DO7" s="26" t="n"/>
-      <c r="DP7" s="26" t="n"/>
-      <c r="DQ7" s="27" t="n"/>
-      <c r="DR7" s="25" t="n"/>
-      <c r="DS7" s="26" t="n"/>
+      <c r="DF7" s="22" t="n"/>
+      <c r="DG7" s="23" t="n"/>
+      <c r="DH7" s="23" t="n"/>
+      <c r="DI7" s="23" t="n"/>
+      <c r="DJ7" s="23" t="n"/>
+      <c r="DK7" s="23" t="n"/>
+      <c r="DL7" s="23" t="n"/>
+      <c r="DM7" s="23" t="n"/>
+      <c r="DN7" s="23" t="n"/>
+      <c r="DO7" s="23" t="n"/>
+      <c r="DP7" s="23" t="n"/>
+      <c r="DQ7" s="24" t="n"/>
+      <c r="DR7" s="22" t="n"/>
+      <c r="DS7" s="23" t="n"/>
       <c r="DT7" s="23" t="n"/>
       <c r="DU7" s="23" t="n"/>
       <c r="DV7" s="23" t="n"/>
@@ -2223,27 +2223,27 @@
       <c r="W8" s="23" t="n"/>
       <c r="X8" s="23" t="n"/>
       <c r="Y8" s="24" t="n"/>
-      <c r="Z8" s="25" t="n"/>
-      <c r="AA8" s="26" t="n"/>
-      <c r="AB8" s="26" t="n"/>
-      <c r="AC8" s="26" t="n"/>
-      <c r="AD8" s="26" t="n"/>
-      <c r="AE8" s="26" t="n"/>
-      <c r="AF8" s="26" t="n"/>
-      <c r="AG8" s="26" t="n"/>
-      <c r="AH8" s="26" t="n"/>
-      <c r="AI8" s="26" t="n"/>
-      <c r="AJ8" s="26" t="n"/>
-      <c r="AK8" s="27" t="n"/>
-      <c r="AL8" s="25" t="n"/>
-      <c r="AM8" s="26" t="n"/>
-      <c r="AN8" s="26" t="n"/>
-      <c r="AO8" s="26" t="n"/>
-      <c r="AP8" s="26" t="n"/>
-      <c r="AQ8" s="26" t="n"/>
-      <c r="AR8" s="26" t="n"/>
-      <c r="AS8" s="26" t="n"/>
-      <c r="AT8" s="26" t="n"/>
+      <c r="Z8" s="22" t="n"/>
+      <c r="AA8" s="23" t="n"/>
+      <c r="AB8" s="23" t="n"/>
+      <c r="AC8" s="23" t="n"/>
+      <c r="AD8" s="23" t="n"/>
+      <c r="AE8" s="23" t="n"/>
+      <c r="AF8" s="23" t="n"/>
+      <c r="AG8" s="23" t="n"/>
+      <c r="AH8" s="23" t="n"/>
+      <c r="AI8" s="23" t="n"/>
+      <c r="AJ8" s="23" t="n"/>
+      <c r="AK8" s="24" t="n"/>
+      <c r="AL8" s="22" t="n"/>
+      <c r="AM8" s="23" t="n"/>
+      <c r="AN8" s="23" t="n"/>
+      <c r="AO8" s="23" t="n"/>
+      <c r="AP8" s="23" t="n"/>
+      <c r="AQ8" s="23" t="n"/>
+      <c r="AR8" s="23" t="n"/>
+      <c r="AS8" s="23" t="n"/>
+      <c r="AT8" s="23" t="n"/>
       <c r="AU8" s="23" t="n"/>
       <c r="AV8" s="23" t="n"/>
       <c r="AW8" s="24" t="n"/>
@@ -2337,45 +2337,45 @@
       <c r="EG8" s="23" t="n"/>
       <c r="EH8" s="23" t="n"/>
       <c r="EI8" s="23" t="n"/>
-      <c r="EJ8" s="26" t="n"/>
-      <c r="EK8" s="26" t="n"/>
-      <c r="EL8" s="26" t="n"/>
-      <c r="EM8" s="26" t="n"/>
-      <c r="EN8" s="26" t="n"/>
-      <c r="EO8" s="27" t="n"/>
-      <c r="EP8" s="25" t="n"/>
-      <c r="EQ8" s="26" t="n"/>
-      <c r="ER8" s="26" t="n"/>
-      <c r="ES8" s="26" t="n"/>
-      <c r="ET8" s="26" t="n"/>
-      <c r="EU8" s="26" t="n"/>
-      <c r="EV8" s="26" t="n"/>
-      <c r="EW8" s="26" t="n"/>
-      <c r="EX8" s="26" t="n"/>
-      <c r="EY8" s="26" t="n"/>
-      <c r="EZ8" s="26" t="n"/>
-      <c r="FA8" s="27" t="n"/>
-      <c r="FB8" s="25" t="n"/>
-      <c r="FC8" s="26" t="n"/>
-      <c r="FD8" s="26" t="n"/>
-      <c r="FE8" s="26" t="n"/>
-      <c r="FF8" s="26" t="n"/>
-      <c r="FG8" s="26" t="n"/>
-      <c r="FH8" s="26" t="n"/>
-      <c r="FI8" s="26" t="n"/>
-      <c r="FJ8" s="26" t="n"/>
-      <c r="FK8" s="26" t="n"/>
-      <c r="FL8" s="26" t="n"/>
-      <c r="FM8" s="27" t="n"/>
-      <c r="FN8" s="25" t="n"/>
-      <c r="FO8" s="26" t="n"/>
-      <c r="FP8" s="26" t="n"/>
-      <c r="FQ8" s="26" t="n"/>
-      <c r="FR8" s="26" t="n"/>
-      <c r="FS8" s="26" t="n"/>
-      <c r="FT8" s="26" t="n"/>
-      <c r="FU8" s="26" t="n"/>
-      <c r="FV8" s="26" t="n"/>
+      <c r="EJ8" s="23" t="n"/>
+      <c r="EK8" s="23" t="n"/>
+      <c r="EL8" s="23" t="n"/>
+      <c r="EM8" s="23" t="n"/>
+      <c r="EN8" s="23" t="n"/>
+      <c r="EO8" s="24" t="n"/>
+      <c r="EP8" s="22" t="n"/>
+      <c r="EQ8" s="23" t="n"/>
+      <c r="ER8" s="23" t="n"/>
+      <c r="ES8" s="23" t="n"/>
+      <c r="ET8" s="23" t="n"/>
+      <c r="EU8" s="23" t="n"/>
+      <c r="EV8" s="23" t="n"/>
+      <c r="EW8" s="23" t="n"/>
+      <c r="EX8" s="23" t="n"/>
+      <c r="EY8" s="23" t="n"/>
+      <c r="EZ8" s="23" t="n"/>
+      <c r="FA8" s="24" t="n"/>
+      <c r="FB8" s="22" t="n"/>
+      <c r="FC8" s="23" t="n"/>
+      <c r="FD8" s="23" t="n"/>
+      <c r="FE8" s="23" t="n"/>
+      <c r="FF8" s="23" t="n"/>
+      <c r="FG8" s="23" t="n"/>
+      <c r="FH8" s="23" t="n"/>
+      <c r="FI8" s="23" t="n"/>
+      <c r="FJ8" s="23" t="n"/>
+      <c r="FK8" s="23" t="n"/>
+      <c r="FL8" s="23" t="n"/>
+      <c r="FM8" s="24" t="n"/>
+      <c r="FN8" s="22" t="n"/>
+      <c r="FO8" s="23" t="n"/>
+      <c r="FP8" s="23" t="n"/>
+      <c r="FQ8" s="23" t="n"/>
+      <c r="FR8" s="23" t="n"/>
+      <c r="FS8" s="23" t="n"/>
+      <c r="FT8" s="23" t="n"/>
+      <c r="FU8" s="23" t="n"/>
+      <c r="FV8" s="23" t="n"/>
       <c r="FW8" s="23" t="n"/>
       <c r="FX8" s="23" t="n"/>
       <c r="FY8" s="24" t="n"/>

</xml_diff>